<commit_message>
Fix library data validation
</commit_message>
<xml_diff>
--- a/coyote_badger/static/Sources.xlsx
+++ b/coyote_badger/static/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsands/Documents/GitHub/coyote-badger/coyote_badger/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59550BA-E019-1A47-90CF-C988D9104E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490AED5D-7BA8-D54B-953D-B8542F13F684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -570,91 +570,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB159FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB159FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <b val="0"/>
@@ -2488,20 +2404,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:K5002" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3051,7 +2967,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36979,29 +36895,26 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K3:K5002 A3:E5002">
-    <cfRule type="expression" dxfId="30" priority="55">
+    <cfRule type="expression" dxfId="18" priority="55">
       <formula>#REF!="Not Available at UT"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="56">
+    <cfRule type="expression" dxfId="17" priority="56">
       <formula>#REF!="Other UT Library"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="57">
+    <cfRule type="expression" dxfId="16" priority="57">
       <formula>#REF!="PCL"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="58">
+    <cfRule type="expression" dxfId="15" priority="58">
       <formula>#REF!="Tarlton - Library Use Only"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="59">
+    <cfRule type="expression" dxfId="14" priority="59">
       <formula>#REF!="Tarlton"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="60">
+    <cfRule type="expression" dxfId="13" priority="60">
       <formula>#REF!="eBook"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H5002 I5003:I1048576" xr:uid="{6A5EF0D3-4864-5E43-83A1-B1123617DC02}">
-      <formula1>"Tarlton,Tarlton - Library Use Only,PCL,Other UT Library,eBook,Not Available at UT"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{061F2A0E-F285-464E-A7E0-D54424F3C2B2}">
       <formula1>"Book,Website,SSRN,Journal,State Statute,Federal Statute,SCOTUS Case,Non-SCOTUS Case,Unknown"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Revert "Fix library data validation"
This reverts commit 8fde3a848dad86b5f4f238b7b9e3096ef4166871.
</commit_message>
<xml_diff>
--- a/coyote_badger/static/Sources.xlsx
+++ b/coyote_badger/static/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsands/Documents/GitHub/coyote-badger/coyote_badger/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490AED5D-7BA8-D54B-953D-B8542F13F684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59550BA-E019-1A47-90CF-C988D9104E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -570,7 +570,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB159FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB159FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2404,20 +2488,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A2:K5002" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2967,7 +3051,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36895,26 +36979,29 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K3:K5002 A3:E5002">
-    <cfRule type="expression" dxfId="18" priority="55">
+    <cfRule type="expression" dxfId="30" priority="55">
       <formula>#REF!="Not Available at UT"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="56">
+    <cfRule type="expression" dxfId="29" priority="56">
       <formula>#REF!="Other UT Library"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="57">
+    <cfRule type="expression" dxfId="28" priority="57">
       <formula>#REF!="PCL"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="58">
+    <cfRule type="expression" dxfId="27" priority="58">
       <formula>#REF!="Tarlton - Library Use Only"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="59">
+    <cfRule type="expression" dxfId="26" priority="59">
       <formula>#REF!="Tarlton"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="60">
+    <cfRule type="expression" dxfId="25" priority="60">
       <formula>#REF!="eBook"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H5002 I5003:I1048576" xr:uid="{6A5EF0D3-4864-5E43-83A1-B1123617DC02}">
+      <formula1>"Tarlton,Tarlton - Library Use Only,PCL,Other UT Library,eBook,Not Available at UT"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{061F2A0E-F285-464E-A7E0-D54424F3C2B2}">
       <formula1>"Book,Website,SSRN,Journal,State Statute,Federal Statute,SCOTUS Case,Non-SCOTUS Case,Unknown"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Update docker run command
</commit_message>
<xml_diff>
--- a/coyote_badger/static/Sources.xlsx
+++ b/coyote_badger/static/Sources.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsands/Documents/GitHub/coyote-badger/coyote_badger/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorlewis/Desktop/coyote-badger/coyote_badger/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59550BA-E019-1A47-90CF-C988D9104E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3938E27E-8751-DF42-A98D-D6E00BF2E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -570,91 +569,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB159FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB159FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <b val="0"/>
@@ -2488,20 +2403,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:K5002" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3038,7 +2953,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -3051,7 +2966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36979,22 +36894,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K3:K5002 A3:E5002">
-    <cfRule type="expression" dxfId="30" priority="55">
+    <cfRule type="expression" dxfId="18" priority="55">
       <formula>#REF!="Not Available at UT"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="56">
+    <cfRule type="expression" dxfId="17" priority="56">
       <formula>#REF!="Other UT Library"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="57">
+    <cfRule type="expression" dxfId="16" priority="57">
       <formula>#REF!="PCL"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="58">
+    <cfRule type="expression" dxfId="15" priority="58">
       <formula>#REF!="Tarlton - Library Use Only"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="59">
+    <cfRule type="expression" dxfId="14" priority="59">
       <formula>#REF!="Tarlton"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="60">
+    <cfRule type="expression" dxfId="13" priority="60">
       <formula>#REF!="eBook"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Support Apple Silicon in development mode (#7)
* Add support for Apple Silicon

* Pull playwright directly in Dockerfile

* Bump python version

* Update docker run command
</commit_message>
<xml_diff>
--- a/coyote_badger/static/Sources.xlsx
+++ b/coyote_badger/static/Sources.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexsands/Documents/GitHub/coyote-badger/coyote_badger/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorlewis/Desktop/coyote-badger/coyote_badger/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59550BA-E019-1A47-90CF-C988D9104E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3938E27E-8751-DF42-A98D-D6E00BF2E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -570,91 +569,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB159FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB159FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <b val="0"/>
@@ -2488,20 +2403,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:K5002" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:K5002" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="19"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Member Name" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D904832F-A966-2647-9466-109EFA6BAA2C}" name="FN#" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{50BBB5BE-3FAD-2C4D-A042-634667107ADA}" name="Citation" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Short Cite" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Source Type" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Book Available?" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Library" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D0805E8F-02A0-B84D-A8ED-36287E1B211B}" name="Call Number" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{26B65AED-5E6F-8943-88DF-08FDC31973AD}" name="Notes for Research Editor " dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{6CA9E383-3740-0A4B-B83F-CF43656A9480}" name="Source Puller Result" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3038,7 +2953,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -3051,7 +2966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36979,22 +36894,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K3:K5002 A3:E5002">
-    <cfRule type="expression" dxfId="30" priority="55">
+    <cfRule type="expression" dxfId="18" priority="55">
       <formula>#REF!="Not Available at UT"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="56">
+    <cfRule type="expression" dxfId="17" priority="56">
       <formula>#REF!="Other UT Library"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="57">
+    <cfRule type="expression" dxfId="16" priority="57">
       <formula>#REF!="PCL"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="58">
+    <cfRule type="expression" dxfId="15" priority="58">
       <formula>#REF!="Tarlton - Library Use Only"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="59">
+    <cfRule type="expression" dxfId="14" priority="59">
       <formula>#REF!="Tarlton"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="60">
+    <cfRule type="expression" dxfId="13" priority="60">
       <formula>#REF!="eBook"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>